<commit_message>
seeding database with new 10 records
</commit_message>
<xml_diff>
--- a/seed_data.xlsx
+++ b/seed_data.xlsx
@@ -421,16 +421,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Goyette, Graham and Langworth</v>
+        <v>Hintz LLC</v>
       </c>
       <c r="B2">
-        <v>1949</v>
+        <v>1763</v>
       </c>
       <c r="C2" t="str">
-        <v>West Sofiaton</v>
+        <v>Jocelynfort</v>
       </c>
       <c r="D2">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E2" t="str">
         <v>Test Case 1</v>
@@ -438,16 +438,16 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Kris and Sons</v>
+        <v>Reichel, Weissnat and Stroman</v>
       </c>
       <c r="B3">
-        <v>1645</v>
+        <v>1618</v>
       </c>
       <c r="C3" t="str">
-        <v>Lemketon</v>
+        <v>Sauerburgh</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="E3" t="str">
         <v>Test Case 2</v>
@@ -455,16 +455,16 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Pfannerstill - Beatty</v>
+        <v>Cormier - Hodkiewicz</v>
       </c>
       <c r="B4">
-        <v>1664</v>
+        <v>1763</v>
       </c>
       <c r="C4" t="str">
-        <v>East Lansing</v>
+        <v>Mariannetown</v>
       </c>
       <c r="D4">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E4" t="str">
         <v>Test Case 3</v>
@@ -472,16 +472,16 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Klocko LLC</v>
+        <v>Armstrong Inc</v>
       </c>
       <c r="B5">
-        <v>1671</v>
+        <v>1809</v>
       </c>
       <c r="C5" t="str">
-        <v>Ralphview</v>
+        <v>Rauview</v>
       </c>
       <c r="D5">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="E5" t="str">
         <v>Test Case 4</v>
@@ -489,16 +489,16 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Turner, Kautzer and Mills</v>
+        <v>Padberg - Bauch</v>
       </c>
       <c r="B6">
-        <v>1819</v>
+        <v>2004</v>
       </c>
       <c r="C6" t="str">
-        <v>West Kayleyton</v>
+        <v>Hillsport</v>
       </c>
       <c r="D6">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E6" t="str">
         <v>Test Case 5</v>
@@ -506,16 +506,16 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Weber - Feil</v>
+        <v>Gutkowski, Mraz and Moore</v>
       </c>
       <c r="B7">
-        <v>1609</v>
+        <v>1874</v>
       </c>
       <c r="C7" t="str">
-        <v>Luciusburgh</v>
+        <v>Round Rock</v>
       </c>
       <c r="D7">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="E7" t="str">
         <v>Test Case 6</v>
@@ -523,16 +523,16 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Ritchie Inc</v>
+        <v>Ziemann - Lesch</v>
       </c>
       <c r="B8">
-        <v>1791</v>
+        <v>1839</v>
       </c>
       <c r="C8" t="str">
-        <v>Idaho Falls</v>
+        <v>Beattyport</v>
       </c>
       <c r="D8">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="E8" t="str">
         <v>Test Case 7</v>
@@ -540,16 +540,16 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Lindgren - Hauck</v>
+        <v>Kuhic - Runte</v>
       </c>
       <c r="B9">
-        <v>1640</v>
+        <v>1645</v>
       </c>
       <c r="C9" t="str">
-        <v>Brandontown</v>
+        <v>Judsonview</v>
       </c>
       <c r="D9">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="E9" t="str">
         <v>Test Case 8</v>
@@ -557,16 +557,16 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>MacGyver Inc</v>
+        <v>Morar - Harvey</v>
       </c>
       <c r="B10">
-        <v>1938</v>
+        <v>1987</v>
       </c>
       <c r="C10" t="str">
-        <v>North Kenyattabury</v>
+        <v>Gorczanytown</v>
       </c>
       <c r="D10">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E10" t="str">
         <v>Test Case 9</v>
@@ -574,16 +574,16 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Welch - Lehner</v>
+        <v>Glover - Rempel</v>
       </c>
       <c r="B11">
-        <v>1775</v>
+        <v>1798</v>
       </c>
       <c r="C11" t="str">
-        <v>Port Imani</v>
+        <v>Goldenburgh</v>
       </c>
       <c r="D11">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E11" t="str">
         <v>Test Case 10</v>

</xml_diff>